<commit_message>
Projeto Clima tempo com melhor organizaçao usando Classes
</commit_message>
<xml_diff>
--- a/historico_temperatura.xlsx
+++ b/historico_temperatura.xlsx
@@ -1,55 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudos\PROGRAMAÇÃO\FACULDADE\aulas\development with Python\projeto-clima-tempo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C444F66-048A-44A4-A32D-74D2FBA26640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="675" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="temperatura" sheetId="1" r:id="rId1"/>
+    <sheet name="temperatura" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>DATA/HORA</t>
-  </si>
-  <si>
-    <t>TEMPERATURA</t>
-  </si>
-  <si>
-    <t>UMIDADE DO AR</t>
-  </si>
-  <si>
-    <t>2024-11-21 19:29:38</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -68,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -348,34 +385,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="30.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>DATA/HORA</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TEMPERATURA</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>UMIDADE DO AR</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-11-21 21:44:29</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-11-21 21:49:33</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Chuvas Intensas</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-11-21 21:50:15</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Chuvas Intensas</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-11-21 21:51:07</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Chuvas Intensas</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criando uma funçao para executar o programa dentro da Classe e prints para mostrar a linha e qual planilha os dados foram salvos
</commit_message>
<xml_diff>
--- a/historico_temperatura.xlsx
+++ b/historico_temperatura.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -475,6 +475,36 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-11-21 22:06:49</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Chuvas Intensas</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-11-21 22:08:04</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>19</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Chuvas Intensas</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tratando erros caso nao encontrar a linha de umidade do ar
</commit_message>
<xml_diff>
--- a/historico_temperatura.xlsx
+++ b/historico_temperatura.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -505,6 +505,46 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-11-21 22:11:45</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Chuvas Intensas</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-11-22 12:22:29</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-11-22 12:23:33</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>21</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alerta Umidade nao encontrado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando a funcionalidade de tela grafica com o Tkinder para usar o app apartir de um botao
</commit_message>
<xml_diff>
--- a/historico_temperatura.xlsx
+++ b/historico_temperatura.xlsx
@@ -1,33 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudos\PROGRAMAÇÃO\FACULDADE\aulas\development with Python\projeto-clima-tempo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49B10EE-01F6-4505-8B13-256E8244DFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="temperatura" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="temperatura" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+  <si>
+    <t>DATA/HORA</t>
+  </si>
+  <si>
+    <t>TEMPERATURA</t>
+  </si>
+  <si>
+    <t>UMIDADE DO AR</t>
+  </si>
+  <si>
+    <t>2024-11-21 21:44:29</t>
+  </si>
+  <si>
+    <t>2024-11-21 21:49:33</t>
+  </si>
+  <si>
+    <t>Alerta Amarelo, Chuvas Intensas</t>
+  </si>
+  <si>
+    <t>2024-11-21 21:50:15</t>
+  </si>
+  <si>
+    <t>2024-11-21 21:51:07</t>
+  </si>
+  <si>
+    <t>2024-11-21 22:06:49</t>
+  </si>
+  <si>
+    <t>2024-11-21 22:08:04</t>
+  </si>
+  <si>
+    <t>2024-11-21 22:11:45</t>
+  </si>
+  <si>
+    <t>2024-11-22 12:22:29</t>
+  </si>
+  <si>
+    <t>2024-11-22 12:23:33</t>
+  </si>
+  <si>
+    <t>Alerta Umidade nao encontrado</t>
+  </si>
+  <si>
+    <t>2024-11-22 12:25:03</t>
+  </si>
+  <si>
+    <t>2024-11-22 12:25:28</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +104,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -385,164 +384,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="18.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="14.140625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="30.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>DATA/HORA</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>TEMPERATURA</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>UMIDADE DO AR</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-11-21 21:44:29</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>20</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-11-21 21:49:33</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>20</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alerta Amarelo, Chuvas Intensas</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-11-21 21:50:15</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alerta Amarelo, Chuvas Intensas</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-11-21 21:51:07</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
         <v>20</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alerta Amarelo, Chuvas Intensas</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-11-21 22:06:49</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alerta Amarelo, Chuvas Intensas</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-11-21 22:08:04</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>19</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alerta Amarelo, Chuvas Intensas</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-11-21 22:11:45</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
         <v>20</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alerta Amarelo, Chuvas Intensas</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-11-22 12:22:29</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
         <v>21</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-11-22 12:23:33</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
         <v>21</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alerta Umidade nao encontrado</t>
-        </is>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dados da planilha att e interface do tkinter
</commit_message>
<xml_diff>
--- a/historico_temperatura.xlsx
+++ b/historico_temperatura.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -590,6 +590,66 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-11-27 18:09:29</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>29</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alerta Umidade nao encontrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-11-27 18:23:12</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>29</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alerta Umidade nao encontrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-11-27 18:45:37</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>31</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alerta Umidade nao encontrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-11-27 18:48:50</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>30</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alerta Umidade nao encontrado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>